<commit_message>
Prep File cleanup continued
</commit_message>
<xml_diff>
--- a/File Legend.xlsx
+++ b/File Legend.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kip Madden\Desktop\dataScience\MortgageML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F605864C-2F8B-4F69-AFC8-7DD55E9EC6AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9370E0A6-0F0E-4453-9BBD-D0DD40AABD04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38505" yWindow="0" windowWidth="38175" windowHeight="20775" activeTab="3" xr2:uid="{5CCB278A-5778-4807-92F6-A80EAE9D3D45}"/>
+    <workbookView xWindow="120" yWindow="420" windowWidth="38175" windowHeight="20775" activeTab="3" xr2:uid="{5CCB278A-5778-4807-92F6-A80EAE9D3D45}"/>
   </bookViews>
   <sheets>
     <sheet name="Aquisition Prep" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="96">
   <si>
     <t>File Name</t>
   </si>
@@ -511,6 +511,27 @@
   </si>
   <si>
     <t>FM_Aquisition_Processing_Refi.ipynb</t>
+  </si>
+  <si>
+    <t>FMAcqProcessedRefi.csv</t>
+  </si>
+  <si>
+    <t>Fill Null values with "0"</t>
+  </si>
+  <si>
+    <t>mortInsTye, pMIperct</t>
+  </si>
+  <si>
+    <t>mortInsTye, pMIperct, origCLTV</t>
+  </si>
+  <si>
+    <t>ML column prep</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>origChannel:R,B,C &gt; 1,2,3  loanPurp: C,R,U &gt; 1,2,3 sellerName: text &gt; numbers propState: text &gt; numbers</t>
   </si>
 </sst>
 </file>
@@ -605,7 +626,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -633,6 +654,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -947,166 +971,221 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A6C953F-51AD-4961-8BBC-583845C83326}">
-  <dimension ref="A1:Q10"/>
+  <dimension ref="A1:R10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.28515625" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="20.42578125" customWidth="1"/>
-    <col min="6" max="6" width="25.140625" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" customWidth="1"/>
-    <col min="8" max="8" width="17.140625" customWidth="1"/>
-    <col min="9" max="9" width="23.28515625" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" customWidth="1"/>
-    <col min="11" max="11" width="35.85546875" customWidth="1"/>
-    <col min="12" max="12" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="32.5703125" customWidth="1"/>
+    <col min="1" max="1" width="22.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.28515625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" style="9" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" style="9" customWidth="1"/>
+    <col min="6" max="6" width="25.140625" style="9" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" style="9" customWidth="1"/>
+    <col min="8" max="8" width="17.140625" style="9" customWidth="1"/>
+    <col min="9" max="9" width="23.28515625" style="9" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" style="9" customWidth="1"/>
+    <col min="11" max="11" width="31.7109375" style="9" customWidth="1"/>
+    <col min="12" max="12" width="35.85546875" style="9" customWidth="1"/>
+    <col min="13" max="13" width="29.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="32.5703125" style="9" customWidth="1"/>
+    <col min="15" max="15" width="27.140625" style="9" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" ht="37.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:18" s="7" customFormat="1" ht="37.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="L1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-    </row>
-    <row r="2" spans="1:17" s="1" customFormat="1" ht="43.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="O1" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+    </row>
+    <row r="2" spans="1:18" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="8">
         <v>10535111</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="L2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="O2" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="8">
         <v>25993874</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="K3" s="11"/>
+      <c r="L3" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="N3" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
+    <row r="4" spans="1:18" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="C4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="O4" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>